<commit_message>
Minor change to BOM details
</commit_message>
<xml_diff>
--- a/SU23 LIGHT MODULE (BOM).xlsx
+++ b/SU23 LIGHT MODULE (BOM).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foohoong.fong\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foohoong.fong\06. [M] 2023 DP TEACHING\37. (2023-5 SU23) MET2001 (SYSTEM PROJECT 1)\PCB\SEP150_LED LIGHT MODULE (V1.1) [SENT 14 APR 23]\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -709,7 +709,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -720,32 +720,33 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="82.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="82.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -863,7 +864,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -922,7 +923,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -981,7 +982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>